<commit_message>
optimization for article pipe
</commit_message>
<xml_diff>
--- a/data/name/client_with_alternative_names.xlsx
+++ b/data/name/client_with_alternative_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Алина\Documents\SberPacharmProjects\FinGigaChat\data\name\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E323F7D-47FB-48E3-9C08-795D0C9DF4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886D4964-20CD-49D4-AD8C-D6A09F79D9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="946">
   <si>
     <t>Клиент</t>
   </si>
@@ -118,9 +118,6 @@
     <t xml:space="preserve"> БВР </t>
   </si>
   <si>
-    <t xml:space="preserve"> Компания БВР </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Capital Partners </t>
   </si>
   <si>
@@ -343,9 +340,6 @@
     <t xml:space="preserve"> Limak </t>
   </si>
   <si>
-    <t xml:space="preserve"> Limak Holding </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Luxoft Company </t>
   </si>
   <si>
@@ -406,9 +400,6 @@
     <t xml:space="preserve"> Multinational logistics partnership </t>
   </si>
   <si>
-    <t xml:space="preserve"> УК MLP </t>
-  </si>
-  <si>
     <t xml:space="preserve"> MR Group </t>
   </si>
   <si>
@@ -445,9 +436,6 @@
     <t xml:space="preserve"> OCS </t>
   </si>
   <si>
-    <t xml:space="preserve"> OCS Distribution </t>
-  </si>
-  <si>
     <t xml:space="preserve"> OZON </t>
   </si>
   <si>
@@ -478,12 +466,6 @@
     <t xml:space="preserve"> Raven Property Group </t>
   </si>
   <si>
-    <t xml:space="preserve"> Raven Russia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Raven Property </t>
-  </si>
-  <si>
     <t xml:space="preserve"> RD Group </t>
   </si>
   <si>
@@ -589,9 +571,6 @@
     <t xml:space="preserve"> АО "ТОРГОВЫЙ ДОМ "ПЕРЕКРЕСТОК" </t>
   </si>
   <si>
-    <t xml:space="preserve"> X5 Group </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Перекресток </t>
   </si>
   <si>
@@ -721,9 +700,6 @@
     <t xml:space="preserve"> КОМКОР </t>
   </si>
   <si>
-    <t xml:space="preserve"> АКАДО Телеком </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Акрон </t>
   </si>
   <si>
@@ -964,9 +940,6 @@
     <t xml:space="preserve"> Сеть магазинов "Верный" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Компания "Верный" </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Верхнебаканский цементный завод </t>
   </si>
   <si>
@@ -1075,15 +1048,9 @@
     <t xml:space="preserve"> АО фирма "Агрокомплекс" имени Н. И. Ткачёв </t>
   </si>
   <si>
-    <t xml:space="preserve"> "Агрокомплекс Выселковский" </t>
-  </si>
-  <si>
     <t xml:space="preserve"> "Агрокомплекс" им. Н.И. Ткачева </t>
   </si>
   <si>
-    <t xml:space="preserve"> АО фирма АГРОКОМПЛЕКС </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ГК Касперский </t>
   </si>
   <si>
@@ -1207,9 +1174,6 @@
     <t xml:space="preserve"> ГК "Доминант" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Группа компаний "Доминант" </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Домус-Тевади </t>
   </si>
   <si>
@@ -1255,9 +1219,6 @@
     <t xml:space="preserve"> ООО "ЗАБАЙКАЛЬСКИЙ ТЕРМИНАЛ" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Забайкальский Зерновой Терминал </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ЗЗТ </t>
   </si>
   <si>
@@ -1636,9 +1597,6 @@
     <t xml:space="preserve"> ПАО "Метафракс" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Биннофарм групп </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Мечел </t>
   </si>
   <si>
@@ -1987,12 +1945,6 @@
     <t xml:space="preserve"> АО "ПРОГРЕСС" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Производственно-торговая компания "Прогресс" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> торговая компания "Прогресс" </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Продимекс </t>
   </si>
   <si>
@@ -2302,9 +2254,6 @@
     <t xml:space="preserve"> СЕТЬ ТЕЛЕВИЗИОННЫХ СТАНЦИЙ </t>
   </si>
   <si>
-    <t xml:space="preserve"> Корпорация СТС </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Сибирский Антрацит </t>
   </si>
   <si>
@@ -2392,9 +2341,6 @@
     <t xml:space="preserve"> ГК "Содружество" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Группа компаний "Содружество" </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ГК Содружество </t>
   </si>
   <si>
@@ -2584,9 +2530,6 @@
     <t xml:space="preserve"> Турухан </t>
   </si>
   <si>
-    <t xml:space="preserve"> Авиакомпания Турухан </t>
-  </si>
-  <si>
     <t xml:space="preserve"> УАЗ </t>
   </si>
   <si>
@@ -2861,6 +2804,60 @@
   </si>
   <si>
     <t xml:space="preserve"> Пятёрочка </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Компания БВР </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Limak Holding </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> УК MLP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OCS Distribution </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Raven Russia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Raven Property </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X5 Group </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Компания "Верный" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Агрокомплекс Выселковский" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> АО фирма АГРОКОМПЛЕКС </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Группа компаний "Доминант" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Забайкальский Зерновой Терминал </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Биннофарм групп </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Производственно-торговая компания "Прогресс" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> торговая компания "Прогресс" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Корпорация СТС </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Группа компаний "Содружество" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Авиакомпания Турухан </t>
   </si>
 </sst>
 </file>
@@ -2916,12 +2913,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3228,8 +3222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="G318" sqref="G318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3268,8 +3262,8 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>945</v>
+      <c r="K1" s="1" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3356,3441 +3350,3441 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>928</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
         <v>59</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>65</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>66</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>67</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
         <v>82</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>86</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>87</v>
-      </c>
-      <c r="E30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
         <v>89</v>
-      </c>
-      <c r="B31" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>92</v>
-      </c>
-      <c r="C32" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
         <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>100</v>
-      </c>
-      <c r="C35" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>104</v>
-      </c>
-      <c r="D36" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>929</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>111</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>112</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>113</v>
-      </c>
-      <c r="E39" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
         <v>118</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>119</v>
-      </c>
-      <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
         <v>122</v>
-      </c>
-      <c r="B42" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" t="s">
         <v>125</v>
       </c>
-      <c r="B43" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" t="s">
-        <v>127</v>
-      </c>
       <c r="D43" t="s">
-        <v>128</v>
+        <v>930</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" t="s">
         <v>133</v>
-      </c>
-      <c r="B46" t="s">
-        <v>134</v>
-      </c>
-      <c r="C46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>931</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>932</v>
       </c>
       <c r="D54" t="s">
-        <v>153</v>
+        <v>933</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C60" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B62" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B65" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B68" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" t="s">
+        <v>934</v>
+      </c>
+      <c r="D69" t="s">
+        <v>183</v>
+      </c>
+      <c r="E69" t="s">
+        <v>184</v>
+      </c>
+      <c r="F69" t="s">
+        <v>185</v>
+      </c>
+      <c r="G69" t="s">
+        <v>186</v>
+      </c>
+      <c r="H69" t="s">
         <v>187</v>
       </c>
-      <c r="B69" t="s">
+      <c r="I69" t="s">
         <v>188</v>
       </c>
-      <c r="C69" t="s">
+      <c r="J69" t="s">
         <v>189</v>
       </c>
-      <c r="D69" t="s">
-        <v>190</v>
-      </c>
-      <c r="E69" t="s">
-        <v>191</v>
-      </c>
-      <c r="F69" t="s">
-        <v>192</v>
-      </c>
-      <c r="G69" t="s">
-        <v>193</v>
-      </c>
-      <c r="H69" t="s">
-        <v>194</v>
-      </c>
-      <c r="I69" t="s">
-        <v>195</v>
-      </c>
-      <c r="J69" t="s">
-        <v>196</v>
-      </c>
       <c r="K69" t="s">
-        <v>946</v>
+        <v>927</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B75" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C75" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B81" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C81" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B82" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C82" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B83" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B85" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B86" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B87" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C87" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D87" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B88" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B90" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C90" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D90" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E90" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C94" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C95" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D95" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B97" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C97" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C98" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C99" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B100" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C100" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B101" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B102" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B103" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C103" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B104" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B105" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B107" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B109" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C109" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D109" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B110" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B111" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C111" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B112" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C112" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B113" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B114" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B115" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B116" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C116" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B117" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B118" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B119" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B120" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B121" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C121" t="s">
-        <v>314</v>
+        <v>935</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B123" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B124" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B125" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C125" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D125" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B126" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>944</v>
+        <v>925</v>
       </c>
       <c r="B127" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C127" t="s">
-        <v>943</v>
+        <v>924</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B128" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C128" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B129" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B130" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B131" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C131" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B132" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C132" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="D132" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="E132" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="F132" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B133" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C133" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B134" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B135" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C135" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D135" t="s">
-        <v>351</v>
+        <v>936</v>
       </c>
       <c r="E135" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="F135" t="s">
-        <v>353</v>
+        <v>937</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="B136" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="B138" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="B139" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="C139" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B140" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B141" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="C141" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="B142" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="C142" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="B143" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="B144" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B146" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="B147" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="B148" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="C148" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="B149" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="B150" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C150" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="D150" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="B151" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="C151" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="B152" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="B153" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C153" t="s">
-        <v>395</v>
+        <v>938</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B154" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="B155" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="C155" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="D155" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="E155" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="B156" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B157" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="B158" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="B159" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="C159" t="s">
-        <v>411</v>
+        <v>939</v>
       </c>
       <c r="D159" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="B160" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="C160" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="B161" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="B162" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="C162" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="B163" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="B164" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="B165" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="B166" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="C166" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="B167" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="B168" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B169" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="B170" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="C170" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="B171" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="B172" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C172" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="B176" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="C176" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="B178" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="C178" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D178" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="E178" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="F178" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="B179" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="C179" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="D179" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="E179" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="B180" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="B182" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="B183" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="B184" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="B185" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C185" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D185" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="E185" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="F185" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="B186" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B187" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="B188" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="B189" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="C189" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="B190" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="C190" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="B191" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="C191" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="B192" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="C192" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="B193" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="C193" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="B194" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="B195" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="C195" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="D195" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="E195" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="B196" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="C196" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="D196" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="E196" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="F196" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="G196" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="B197" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="B198" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="B199" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="B200" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="B201" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="B202" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="B203" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="C203" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="B204" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="B205" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="C205" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="D205" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="E205" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="F205" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="G205" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="B206" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="C206" t="s">
-        <v>538</v>
+        <v>940</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="B207" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="C207" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="D207" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="B208" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="B209" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C209" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="D209" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="E209" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="F209" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="B211" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="C211" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="B212" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="B213" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C213" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="B214" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="C214" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="D214" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="B215" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="B217" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="B218" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="B219" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="C219" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="B220" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="C220" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="D220" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B221" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="C221" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="B222" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="C222" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="D222" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="E222" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="F222" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="G222" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="H222" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="B223" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="B224" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B225" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="C225" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="D225" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="E225" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="F225" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="B226" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="C226" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="B227" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="C227" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="B228" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="B229" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="C229" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="B231" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="C231" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="D231" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="E231" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="F231" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="G231" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="B232" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="B234" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C234" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="B235" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="C235" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="B236" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="C236" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="B237" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="B238" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="C238" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="D238" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="B239" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="C239" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="D239" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="B240" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="C240" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="D240" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
       <c r="B241" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
       <c r="C241" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
       <c r="D241" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="B242" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="B243" t="s">
-        <v>651</v>
+        <v>637</v>
       </c>
       <c r="C243" t="s">
-        <v>652</v>
+        <v>638</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
       <c r="B244" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="C244" t="s">
-        <v>655</v>
+        <v>941</v>
       </c>
       <c r="D244" t="s">
-        <v>656</v>
+        <v>942</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="B245" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="B246" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
       <c r="C246" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="B247" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="C247" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="B248" t="s">
-        <v>666</v>
+        <v>650</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="B249" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="B250" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="C250" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="B252" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="B253" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="B254" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
       <c r="C254" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
       <c r="B255" t="s">
-        <v>681</v>
+        <v>665</v>
       </c>
       <c r="C255" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
       <c r="D255" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>684</v>
+        <v>668</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>685</v>
+        <v>669</v>
       </c>
       <c r="B257" t="s">
-        <v>686</v>
+        <v>670</v>
       </c>
       <c r="C257" t="s">
-        <v>687</v>
+        <v>671</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>688</v>
+        <v>672</v>
       </c>
       <c r="B258" t="s">
-        <v>689</v>
+        <v>673</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>690</v>
+        <v>674</v>
       </c>
       <c r="B259" t="s">
-        <v>691</v>
+        <v>675</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>692</v>
+        <v>676</v>
       </c>
       <c r="B260" t="s">
-        <v>693</v>
+        <v>677</v>
       </c>
       <c r="C260" t="s">
-        <v>694</v>
+        <v>678</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>695</v>
+        <v>679</v>
       </c>
       <c r="B261" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>697</v>
+        <v>681</v>
       </c>
       <c r="B262" t="s">
-        <v>698</v>
+        <v>682</v>
       </c>
       <c r="C262" t="s">
-        <v>699</v>
+        <v>683</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>700</v>
+        <v>684</v>
       </c>
       <c r="B263" t="s">
-        <v>701</v>
+        <v>685</v>
       </c>
       <c r="C263" t="s">
-        <v>702</v>
+        <v>686</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="B264" t="s">
-        <v>704</v>
+        <v>688</v>
       </c>
       <c r="C264" t="s">
-        <v>705</v>
+        <v>689</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>706</v>
+        <v>690</v>
       </c>
       <c r="B265" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="C265" t="s">
-        <v>708</v>
+        <v>692</v>
       </c>
       <c r="D265" t="s">
-        <v>709</v>
+        <v>693</v>
       </c>
       <c r="E265" t="s">
-        <v>710</v>
+        <v>694</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>711</v>
+        <v>695</v>
       </c>
       <c r="B266" t="s">
-        <v>712</v>
+        <v>696</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>713</v>
+        <v>697</v>
       </c>
       <c r="B267" t="s">
-        <v>714</v>
+        <v>698</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="B268" t="s">
-        <v>716</v>
+        <v>700</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>717</v>
+        <v>701</v>
       </c>
       <c r="B269" t="s">
-        <v>718</v>
+        <v>702</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>719</v>
+        <v>703</v>
       </c>
       <c r="B270" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="C270" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>722</v>
+        <v>706</v>
       </c>
       <c r="B271" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>724</v>
+        <v>708</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>725</v>
+        <v>709</v>
       </c>
       <c r="B273" t="s">
-        <v>726</v>
+        <v>710</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>727</v>
+        <v>711</v>
       </c>
       <c r="B274" t="s">
-        <v>728</v>
+        <v>712</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>729</v>
+        <v>713</v>
       </c>
       <c r="B275" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>731</v>
+        <v>715</v>
       </c>
       <c r="B276" t="s">
-        <v>732</v>
+        <v>716</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="B277" t="s">
-        <v>734</v>
+        <v>718</v>
       </c>
       <c r="C277" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="B279" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
       <c r="B280" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>741</v>
+        <v>725</v>
       </c>
       <c r="B281" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
       <c r="C281" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>744</v>
+        <v>728</v>
       </c>
       <c r="B282" t="s">
-        <v>745</v>
+        <v>729</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>746</v>
+        <v>730</v>
       </c>
       <c r="B283" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="C283" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
       <c r="D283" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>750</v>
+        <v>734</v>
       </c>
       <c r="B284" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
       <c r="C284" t="s">
-        <v>752</v>
+        <v>736</v>
       </c>
       <c r="D284" t="s">
-        <v>753</v>
+        <v>737</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>754</v>
+        <v>738</v>
       </c>
       <c r="B285" t="s">
-        <v>755</v>
+        <v>739</v>
       </c>
       <c r="C285" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
       <c r="D285" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="E285" t="s">
-        <v>758</v>
+        <v>742</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>759</v>
+        <v>743</v>
       </c>
       <c r="B286" t="s">
-        <v>760</v>
+        <v>943</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
       <c r="B287" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
       <c r="C287" t="s">
-        <v>763</v>
+        <v>746</v>
       </c>
       <c r="D287" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>765</v>
+        <v>748</v>
       </c>
       <c r="B288" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
       <c r="C288" t="s">
-        <v>767</v>
+        <v>750</v>
       </c>
       <c r="D288" t="s">
-        <v>768</v>
+        <v>751</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
       <c r="B289" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
       <c r="C289" t="s">
-        <v>771</v>
+        <v>754</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>773</v>
+        <v>756</v>
       </c>
       <c r="B291" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>775</v>
+        <v>758</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
       <c r="B293" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="B294" t="s">
-        <v>779</v>
+        <v>762</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="B295" t="s">
-        <v>781</v>
+        <v>764</v>
       </c>
       <c r="C295" t="s">
-        <v>782</v>
+        <v>765</v>
       </c>
       <c r="D295" t="s">
-        <v>783</v>
+        <v>766</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
       <c r="B296" t="s">
-        <v>785</v>
+        <v>768</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
       <c r="B297" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
       <c r="B298" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
       <c r="C298" t="s">
-        <v>790</v>
+        <v>944</v>
       </c>
       <c r="D298" t="s">
-        <v>791</v>
+        <v>773</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>792</v>
+        <v>774</v>
       </c>
       <c r="B299" t="s">
-        <v>793</v>
+        <v>775</v>
       </c>
       <c r="C299" t="s">
-        <v>794</v>
+        <v>776</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>795</v>
+        <v>777</v>
       </c>
       <c r="B300" t="s">
-        <v>796</v>
+        <v>778</v>
       </c>
       <c r="C300" t="s">
-        <v>797</v>
+        <v>779</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>798</v>
+        <v>780</v>
       </c>
       <c r="B301" t="s">
-        <v>799</v>
+        <v>781</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>800</v>
+        <v>782</v>
       </c>
       <c r="B302" t="s">
-        <v>801</v>
+        <v>783</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>802</v>
+        <v>784</v>
       </c>
       <c r="B303" t="s">
-        <v>803</v>
+        <v>785</v>
       </c>
       <c r="C303" t="s">
-        <v>804</v>
+        <v>786</v>
       </c>
       <c r="D303" t="s">
-        <v>805</v>
+        <v>787</v>
       </c>
       <c r="E303" t="s">
-        <v>806</v>
+        <v>788</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>807</v>
+        <v>789</v>
       </c>
       <c r="B304" t="s">
-        <v>808</v>
+        <v>790</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>809</v>
+        <v>791</v>
       </c>
       <c r="B305" t="s">
-        <v>810</v>
+        <v>792</v>
       </c>
       <c r="C305" t="s">
-        <v>811</v>
+        <v>793</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="B306" t="s">
-        <v>813</v>
+        <v>795</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>814</v>
+        <v>796</v>
       </c>
       <c r="B307" t="s">
-        <v>815</v>
+        <v>797</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>816</v>
+        <v>798</v>
       </c>
       <c r="B308" t="s">
-        <v>817</v>
+        <v>799</v>
       </c>
       <c r="C308" t="s">
-        <v>818</v>
+        <v>800</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>819</v>
+        <v>801</v>
       </c>
       <c r="B309" t="s">
-        <v>820</v>
+        <v>802</v>
       </c>
       <c r="C309" t="s">
-        <v>821</v>
+        <v>803</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>822</v>
+        <v>804</v>
       </c>
       <c r="B310" t="s">
-        <v>823</v>
+        <v>805</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>824</v>
+        <v>806</v>
       </c>
       <c r="B311" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
       <c r="C311" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="B312" t="s">
-        <v>828</v>
+        <v>810</v>
       </c>
       <c r="C312" t="s">
-        <v>829</v>
+        <v>811</v>
       </c>
       <c r="D312" t="s">
-        <v>830</v>
+        <v>812</v>
       </c>
       <c r="E312" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="F312" t="s">
-        <v>832</v>
+        <v>814</v>
       </c>
       <c r="G312" t="s">
-        <v>833</v>
+        <v>815</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
       <c r="B313" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="B314" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="B315" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="B316" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="B317" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="C317" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="B318" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>847</v>
+        <v>829</v>
       </c>
       <c r="B319" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="B320" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>851</v>
+        <v>833</v>
       </c>
       <c r="B321" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>853</v>
+        <v>835</v>
       </c>
       <c r="B322" t="s">
-        <v>854</v>
+        <v>945</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>855</v>
+        <v>836</v>
       </c>
       <c r="B323" t="s">
-        <v>856</v>
+        <v>837</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>857</v>
+        <v>838</v>
       </c>
       <c r="B324" t="s">
-        <v>858</v>
+        <v>839</v>
       </c>
       <c r="C324" t="s">
-        <v>859</v>
+        <v>840</v>
       </c>
       <c r="D324" t="s">
-        <v>860</v>
+        <v>841</v>
       </c>
       <c r="E324" t="s">
-        <v>861</v>
+        <v>842</v>
       </c>
       <c r="F324" t="s">
-        <v>862</v>
+        <v>843</v>
       </c>
       <c r="G324" t="s">
-        <v>863</v>
+        <v>844</v>
       </c>
       <c r="H324" t="s">
-        <v>864</v>
+        <v>845</v>
       </c>
       <c r="I324" t="s">
-        <v>865</v>
+        <v>846</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>866</v>
+        <v>847</v>
       </c>
       <c r="B325" t="s">
-        <v>867</v>
+        <v>848</v>
       </c>
       <c r="C325" t="s">
-        <v>868</v>
+        <v>849</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>869</v>
+        <v>850</v>
       </c>
       <c r="B326" t="s">
-        <v>870</v>
+        <v>851</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>871</v>
+        <v>852</v>
       </c>
       <c r="B327" t="s">
-        <v>872</v>
+        <v>853</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>873</v>
+        <v>854</v>
       </c>
       <c r="B328" t="s">
-        <v>874</v>
+        <v>855</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="B329" t="s">
-        <v>876</v>
+        <v>857</v>
       </c>
       <c r="C329" t="s">
-        <v>877</v>
+        <v>858</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>878</v>
+        <v>859</v>
       </c>
       <c r="B330" t="s">
-        <v>879</v>
+        <v>860</v>
       </c>
       <c r="C330" t="s">
-        <v>880</v>
+        <v>861</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>881</v>
+        <v>862</v>
       </c>
       <c r="B331" t="s">
-        <v>882</v>
+        <v>863</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>883</v>
+        <v>864</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>884</v>
+        <v>865</v>
       </c>
       <c r="B333" t="s">
-        <v>885</v>
+        <v>866</v>
       </c>
       <c r="C333" t="s">
-        <v>886</v>
+        <v>867</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>887</v>
+        <v>868</v>
       </c>
       <c r="B334" t="s">
-        <v>888</v>
+        <v>869</v>
       </c>
       <c r="C334" t="s">
-        <v>889</v>
+        <v>870</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>890</v>
+        <v>871</v>
       </c>
       <c r="B335" t="s">
-        <v>891</v>
+        <v>872</v>
       </c>
       <c r="C335" t="s">
-        <v>892</v>
+        <v>873</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>893</v>
+        <v>874</v>
       </c>
       <c r="B336" t="s">
-        <v>894</v>
+        <v>875</v>
       </c>
       <c r="C336" t="s">
-        <v>895</v>
+        <v>876</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>896</v>
+        <v>877</v>
       </c>
       <c r="B337" t="s">
-        <v>897</v>
+        <v>878</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>898</v>
+        <v>879</v>
       </c>
       <c r="B338" t="s">
-        <v>899</v>
+        <v>880</v>
       </c>
       <c r="C338" t="s">
-        <v>900</v>
+        <v>881</v>
       </c>
       <c r="D338" t="s">
-        <v>901</v>
+        <v>882</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>902</v>
+        <v>883</v>
       </c>
       <c r="B339" t="s">
-        <v>903</v>
+        <v>884</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>904</v>
+        <v>885</v>
       </c>
       <c r="B340" t="s">
-        <v>905</v>
+        <v>886</v>
       </c>
       <c r="C340" t="s">
-        <v>906</v>
+        <v>887</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>907</v>
+        <v>888</v>
       </c>
       <c r="B341" t="s">
-        <v>908</v>
+        <v>889</v>
       </c>
       <c r="C341" t="s">
-        <v>909</v>
+        <v>890</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>910</v>
+        <v>891</v>
       </c>
       <c r="B342" t="s">
-        <v>911</v>
+        <v>892</v>
       </c>
       <c r="C342" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>913</v>
+        <v>894</v>
       </c>
       <c r="B343" t="s">
-        <v>914</v>
+        <v>895</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>915</v>
+        <v>896</v>
       </c>
       <c r="B345" t="s">
-        <v>916</v>
+        <v>897</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>917</v>
+        <v>898</v>
       </c>
       <c r="B346" t="s">
-        <v>918</v>
+        <v>899</v>
       </c>
       <c r="C346" t="s">
-        <v>919</v>
+        <v>900</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>920</v>
+        <v>901</v>
       </c>
       <c r="B347" t="s">
-        <v>921</v>
+        <v>902</v>
       </c>
       <c r="C347" t="s">
-        <v>922</v>
+        <v>903</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>923</v>
+        <v>904</v>
       </c>
       <c r="B348" t="s">
-        <v>924</v>
+        <v>905</v>
       </c>
       <c r="C348" t="s">
-        <v>925</v>
+        <v>906</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>926</v>
+        <v>907</v>
       </c>
       <c r="B349" t="s">
-        <v>927</v>
+        <v>908</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>928</v>
+        <v>909</v>
       </c>
       <c r="B350" t="s">
-        <v>929</v>
+        <v>910</v>
       </c>
       <c r="C350" t="s">
-        <v>930</v>
+        <v>911</v>
       </c>
       <c r="D350" t="s">
-        <v>931</v>
+        <v>912</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>932</v>
+        <v>913</v>
       </c>
       <c r="B351" t="s">
-        <v>933</v>
+        <v>914</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>934</v>
+        <v>915</v>
       </c>
       <c r="B352" t="s">
-        <v>935</v>
+        <v>916</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>936</v>
+        <v>917</v>
       </c>
       <c r="B353" t="s">
-        <v>937</v>
+        <v>918</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>938</v>
+        <v>919</v>
       </c>
       <c r="B354" t="s">
-        <v>939</v>
+        <v>920</v>
       </c>
       <c r="C354" t="s">
-        <v>940</v>
+        <v>921</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>941</v>
+        <v>922</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>942</v>
+        <v>923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update search client names in article
</commit_message>
<xml_diff>
--- a/data/name/client_with_alternative_names.xlsx
+++ b/data/name/client_with_alternative_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Алина\Documents\SberPacharmProjects\FinGigaChat\data\name\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886D4964-20CD-49D4-AD8C-D6A09F79D9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF08E40-AF36-4FB7-ADE8-715CF6383943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="948">
   <si>
     <t>Клиент</t>
   </si>
@@ -2858,6 +2858,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Авиакомпания Турухан </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Газпрома </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Газпром нефти </t>
   </si>
 </sst>
 </file>
@@ -3222,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="G318" sqref="G318"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4504,6 +4510,9 @@
       <c r="B130" t="s">
         <v>324</v>
       </c>
+      <c r="C130" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
@@ -4514,6 +4523,9 @@
       </c>
       <c r="C131" t="s">
         <v>327</v>
+      </c>
+      <c r="D131" t="s">
+        <v>947</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
bug fix and update client_with_alternative_names.xlsx
</commit_message>
<xml_diff>
--- a/data/name/client_with_alternative_names.xlsx
+++ b/data/name/client_with_alternative_names.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Алина\Documents\SberPacharmProjects\FinGigaChat\data\name\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D504CCF-AA07-4FCF-B02A-2D3A0D5045A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF73E8B-CA53-42EC-BA0D-0890B3FBD07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="1013">
   <si>
     <t>Клиент</t>
   </si>
@@ -1993,9 +2006,6 @@
     <t xml:space="preserve"> РЗ Агро </t>
   </si>
   <si>
-    <t xml:space="preserve"> РКС </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Российские коммунальные системы </t>
   </si>
   <si>
@@ -2500,9 +2510,6 @@
     <t xml:space="preserve"> ПАО "Центр по перевозке грузов в контейнерах "ТрансКонтейнер" </t>
   </si>
   <si>
-    <t xml:space="preserve"> Группа Дело </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Транснефть </t>
   </si>
   <si>
@@ -2951,6 +2958,120 @@
   </si>
   <si>
     <t xml:space="preserve"> McKinsey </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Порт Тамань </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Аммиакопровод </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ОАО "Верхнебаканский цементный завод" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ВБЦЗ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ГАЗМЕТАЛЛПРОЕКТ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cemros </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> СМИКОМ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> МКСМ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ГК ПРОТЕК </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Протек </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> СОТЕКС </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Центр внедрения ПРОТЕК </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> РАФАРМ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> АПТЕКИ РИГЛА </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ХАЙДЕЛЬБЕРГ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ХАЙДЕЛЬБЕРГЦЕМЕНТ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heidelbergcement </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "СЛАНЦЕВСКИЙ ЦЕМЕНТНЫЙ ЗАВОД "ЦЕСЛА" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ХАЙДЕЛЬБЕРГЦЕМЕНТ РУС" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> АКЦИОНЕРНОЕ ОБЩЕСТВО "НОВАЯ ГРУППА" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HolcimLafarge </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Независимая нефтегазовая компания </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Сургутнефтегаз </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Беларуськалий </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ОАО "Беларуськалий" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ПАО "Сургутнефтегаз" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ЛАФАРЖ ГЕО" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> АО ННК-Приморнефтепродукт </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Белорусская калийная компания </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ННК-Хабаровскнефтепродукт </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ЛАФАРЖ НЕРУДНЫЕ МАТЕРИАЛЫ И БЕТОН" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ХОЛСИМ (РУС) СТРОИТЕЛЬНЫЕ МАТЕРИАЛЫ" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ННК-Амурнефтепродукт </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ННК </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ХОЛСИМ (РУС)" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ЛАФАРЖ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "НОРЦЕМ КОЛА" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ГУРОВО-БЕТОН </t>
   </si>
 </sst>
 </file>
@@ -3313,10 +3434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K354"/>
+  <dimension ref="A1:K363"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3366,7 +3487,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3453,7 +3574,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3502,7 +3623,7 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3598,7 +3719,7 @@
         <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3738,7 +3859,7 @@
         <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3813,7 +3934,7 @@
         <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3864,7 +3985,7 @@
         <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -3886,7 +4007,7 @@
         <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -3910,10 +4031,10 @@
         <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D54" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3989,7 +4110,7 @@
         <v>166</v>
       </c>
       <c r="C62" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -4054,7 +4175,7 @@
         <v>182</v>
       </c>
       <c r="C69" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D69" t="s">
         <v>183</v>
@@ -4078,7 +4199,7 @@
         <v>189</v>
       </c>
       <c r="K69" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -4431,7 +4552,7 @@
         <v>278</v>
       </c>
       <c r="E109" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -4472,7 +4593,7 @@
         <v>288</v>
       </c>
       <c r="C113" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -4510,13 +4631,13 @@
         <v>297</v>
       </c>
       <c r="C117" t="s">
+        <v>857</v>
+      </c>
+      <c r="D117" t="s">
+        <v>858</v>
+      </c>
+      <c r="E117" t="s">
         <v>859</v>
-      </c>
-      <c r="D117" t="s">
-        <v>860</v>
-      </c>
-      <c r="E117" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -4551,10 +4672,10 @@
         <v>305</v>
       </c>
       <c r="C121" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D121" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -4602,13 +4723,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B127" t="s">
         <v>317</v>
       </c>
       <c r="C127" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -4638,7 +4759,7 @@
         <v>324</v>
       </c>
       <c r="C130" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -4652,7 +4773,7 @@
         <v>327</v>
       </c>
       <c r="D131" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -4705,13 +4826,13 @@
         <v>341</v>
       </c>
       <c r="D135" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E135" t="s">
         <v>342</v>
       </c>
       <c r="F135" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -4857,10 +4978,10 @@
         <v>379</v>
       </c>
       <c r="D151" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="E151" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -4871,7 +4992,7 @@
         <v>381</v>
       </c>
       <c r="C152" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -4882,7 +5003,7 @@
         <v>383</v>
       </c>
       <c r="C153" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -4925,6 +5046,9 @@
       <c r="B157" t="s">
         <v>394</v>
       </c>
+      <c r="C157" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
@@ -4933,6 +5057,9 @@
       <c r="B158" t="s">
         <v>396</v>
       </c>
+      <c r="C158" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
@@ -4942,7 +5069,7 @@
         <v>398</v>
       </c>
       <c r="C159" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D159" t="s">
         <v>399</v>
@@ -5216,7 +5343,7 @@
         <v>469</v>
       </c>
       <c r="C188" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -5282,13 +5409,13 @@
         <v>486</v>
       </c>
       <c r="C194" t="s">
+        <v>957</v>
+      </c>
+      <c r="D194" t="s">
+        <v>958</v>
+      </c>
+      <c r="E194" t="s">
         <v>959</v>
-      </c>
-      <c r="D194" t="s">
-        <v>960</v>
-      </c>
-      <c r="E194" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -5429,7 +5556,7 @@
         <v>524</v>
       </c>
       <c r="C206" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -5691,10 +5818,10 @@
         <v>595</v>
       </c>
       <c r="D229" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E229" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -5702,7 +5829,7 @@
         <v>596</v>
       </c>
       <c r="B230" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -5865,10 +5992,10 @@
         <v>640</v>
       </c>
       <c r="C244" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D244" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
@@ -5937,1043 +6064,1202 @@
       <c r="A252" t="s">
         <v>657</v>
       </c>
-      <c r="B252" t="s">
-        <v>658</v>
-      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>658</v>
+      </c>
+      <c r="B253" t="s">
         <v>659</v>
-      </c>
-      <c r="B253" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
+        <v>660</v>
+      </c>
+      <c r="B254" t="s">
         <v>661</v>
       </c>
-      <c r="B254" t="s">
+      <c r="C254" t="s">
         <v>662</v>
-      </c>
-      <c r="C254" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
+        <v>663</v>
+      </c>
+      <c r="B255" t="s">
         <v>664</v>
       </c>
-      <c r="B255" t="s">
+      <c r="C255" t="s">
         <v>665</v>
       </c>
-      <c r="C255" t="s">
+      <c r="D255" t="s">
         <v>666</v>
-      </c>
-      <c r="D255" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
+        <v>668</v>
+      </c>
+      <c r="B257" t="s">
         <v>669</v>
       </c>
-      <c r="B257" t="s">
+      <c r="C257" t="s">
         <v>670</v>
-      </c>
-      <c r="C257" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
+        <v>671</v>
+      </c>
+      <c r="B258" t="s">
         <v>672</v>
-      </c>
-      <c r="B258" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
+        <v>673</v>
+      </c>
+      <c r="B259" t="s">
         <v>674</v>
-      </c>
-      <c r="B259" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
+        <v>675</v>
+      </c>
+      <c r="B260" t="s">
         <v>676</v>
       </c>
-      <c r="B260" t="s">
+      <c r="C260" t="s">
         <v>677</v>
-      </c>
-      <c r="C260" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
+        <v>678</v>
+      </c>
+      <c r="B261" t="s">
         <v>679</v>
-      </c>
-      <c r="B261" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
+        <v>680</v>
+      </c>
+      <c r="B262" t="s">
         <v>681</v>
       </c>
-      <c r="B262" t="s">
+      <c r="C262" t="s">
         <v>682</v>
-      </c>
-      <c r="C262" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
+        <v>683</v>
+      </c>
+      <c r="B263" t="s">
         <v>684</v>
       </c>
-      <c r="B263" t="s">
+      <c r="C263" t="s">
         <v>685</v>
-      </c>
-      <c r="C263" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
+        <v>686</v>
+      </c>
+      <c r="B264" t="s">
         <v>687</v>
       </c>
-      <c r="B264" t="s">
+      <c r="C264" t="s">
         <v>688</v>
-      </c>
-      <c r="C264" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
+        <v>689</v>
+      </c>
+      <c r="B265" t="s">
         <v>690</v>
       </c>
-      <c r="B265" t="s">
+      <c r="C265" t="s">
         <v>691</v>
       </c>
-      <c r="C265" t="s">
+      <c r="D265" t="s">
         <v>692</v>
       </c>
-      <c r="D265" t="s">
+      <c r="E265" t="s">
         <v>693</v>
-      </c>
-      <c r="E265" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
+        <v>694</v>
+      </c>
+      <c r="B266" t="s">
         <v>695</v>
-      </c>
-      <c r="B266" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
+        <v>696</v>
+      </c>
+      <c r="B267" t="s">
         <v>697</v>
       </c>
-      <c r="B267" t="s">
-        <v>698</v>
-      </c>
       <c r="C267" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D267" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
+        <v>698</v>
+      </c>
+      <c r="B268" t="s">
         <v>699</v>
-      </c>
-      <c r="B268" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
+        <v>700</v>
+      </c>
+      <c r="B269" t="s">
         <v>701</v>
-      </c>
-      <c r="B269" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
+        <v>702</v>
+      </c>
+      <c r="B270" t="s">
         <v>703</v>
       </c>
-      <c r="B270" t="s">
+      <c r="C270" t="s">
         <v>704</v>
-      </c>
-      <c r="C270" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
+        <v>705</v>
+      </c>
+      <c r="B271" t="s">
         <v>706</v>
-      </c>
-      <c r="B271" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
+        <v>708</v>
+      </c>
+      <c r="B273" t="s">
         <v>709</v>
-      </c>
-      <c r="B273" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
+        <v>710</v>
+      </c>
+      <c r="B274" t="s">
         <v>711</v>
-      </c>
-      <c r="B274" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
+        <v>712</v>
+      </c>
+      <c r="B275" t="s">
         <v>713</v>
-      </c>
-      <c r="B275" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
+        <v>714</v>
+      </c>
+      <c r="B276" t="s">
         <v>715</v>
-      </c>
-      <c r="B276" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>716</v>
+      </c>
+      <c r="B277" t="s">
         <v>717</v>
       </c>
-      <c r="B277" t="s">
+      <c r="C277" t="s">
         <v>718</v>
-      </c>
-      <c r="C277" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B278" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
+        <v>720</v>
+      </c>
+      <c r="B279" t="s">
         <v>721</v>
-      </c>
-      <c r="B279" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
+        <v>722</v>
+      </c>
+      <c r="B280" t="s">
         <v>723</v>
-      </c>
-      <c r="B280" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>724</v>
+      </c>
+      <c r="B281" t="s">
         <v>725</v>
       </c>
-      <c r="B281" t="s">
+      <c r="C281" t="s">
         <v>726</v>
-      </c>
-      <c r="C281" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
+        <v>727</v>
+      </c>
+      <c r="B282" t="s">
         <v>728</v>
-      </c>
-      <c r="B282" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>729</v>
+      </c>
+      <c r="B283" t="s">
         <v>730</v>
       </c>
-      <c r="B283" t="s">
+      <c r="C283" t="s">
         <v>731</v>
       </c>
-      <c r="C283" t="s">
+      <c r="D283" t="s">
         <v>732</v>
-      </c>
-      <c r="D283" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
+        <v>733</v>
+      </c>
+      <c r="B284" t="s">
         <v>734</v>
       </c>
-      <c r="B284" t="s">
+      <c r="C284" t="s">
         <v>735</v>
       </c>
-      <c r="C284" t="s">
+      <c r="D284" t="s">
         <v>736</v>
-      </c>
-      <c r="D284" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
+        <v>737</v>
+      </c>
+      <c r="B285" t="s">
         <v>738</v>
       </c>
-      <c r="B285" t="s">
+      <c r="C285" t="s">
         <v>739</v>
       </c>
-      <c r="C285" t="s">
+      <c r="D285" t="s">
         <v>740</v>
       </c>
-      <c r="D285" t="s">
+      <c r="E285" t="s">
         <v>741</v>
-      </c>
-      <c r="E285" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B286" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
+        <v>743</v>
+      </c>
+      <c r="B287" t="s">
         <v>744</v>
       </c>
-      <c r="B287" t="s">
+      <c r="C287" t="s">
         <v>745</v>
       </c>
-      <c r="C287" t="s">
+      <c r="D287" t="s">
         <v>746</v>
-      </c>
-      <c r="D287" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
+        <v>747</v>
+      </c>
+      <c r="B288" t="s">
         <v>748</v>
       </c>
-      <c r="B288" t="s">
+      <c r="C288" t="s">
         <v>749</v>
       </c>
-      <c r="C288" t="s">
+      <c r="D288" t="s">
         <v>750</v>
-      </c>
-      <c r="D288" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
+        <v>751</v>
+      </c>
+      <c r="B289" t="s">
         <v>752</v>
       </c>
-      <c r="B289" t="s">
+      <c r="C289" t="s">
         <v>753</v>
-      </c>
-      <c r="C289" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
+        <v>755</v>
+      </c>
+      <c r="B291" t="s">
         <v>756</v>
-      </c>
-      <c r="B291" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B292" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
+        <v>758</v>
+      </c>
+      <c r="B293" t="s">
         <v>759</v>
-      </c>
-      <c r="B293" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
+        <v>760</v>
+      </c>
+      <c r="B294" t="s">
         <v>761</v>
-      </c>
-      <c r="B294" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
+        <v>762</v>
+      </c>
+      <c r="B295" t="s">
         <v>763</v>
       </c>
-      <c r="B295" t="s">
+      <c r="C295" t="s">
         <v>764</v>
       </c>
-      <c r="C295" t="s">
+      <c r="D295" t="s">
         <v>765</v>
-      </c>
-      <c r="D295" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
+        <v>766</v>
+      </c>
+      <c r="B296" t="s">
         <v>767</v>
-      </c>
-      <c r="B296" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
+        <v>768</v>
+      </c>
+      <c r="B297" t="s">
         <v>769</v>
-      </c>
-      <c r="B297" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
+        <v>770</v>
+      </c>
+      <c r="B298" t="s">
         <v>771</v>
       </c>
-      <c r="B298" t="s">
+      <c r="C298" t="s">
+        <v>942</v>
+      </c>
+      <c r="D298" t="s">
         <v>772</v>
-      </c>
-      <c r="C298" t="s">
-        <v>944</v>
-      </c>
-      <c r="D298" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>773</v>
+      </c>
+      <c r="B299" t="s">
         <v>774</v>
       </c>
-      <c r="B299" t="s">
+      <c r="C299" t="s">
         <v>775</v>
-      </c>
-      <c r="C299" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
+        <v>776</v>
+      </c>
+      <c r="B300" t="s">
         <v>777</v>
       </c>
-      <c r="B300" t="s">
+      <c r="C300" t="s">
         <v>778</v>
-      </c>
-      <c r="C300" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
+        <v>779</v>
+      </c>
+      <c r="B301" t="s">
         <v>780</v>
       </c>
-      <c r="B301" t="s">
-        <v>781</v>
-      </c>
       <c r="C301" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D301" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
+        <v>781</v>
+      </c>
+      <c r="B302" t="s">
         <v>782</v>
-      </c>
-      <c r="B302" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
+        <v>783</v>
+      </c>
+      <c r="B303" t="s">
         <v>784</v>
       </c>
-      <c r="B303" t="s">
+      <c r="C303" t="s">
         <v>785</v>
       </c>
-      <c r="C303" t="s">
+      <c r="D303" t="s">
         <v>786</v>
       </c>
-      <c r="D303" t="s">
+      <c r="E303" t="s">
         <v>787</v>
-      </c>
-      <c r="E303" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
+        <v>788</v>
+      </c>
+      <c r="B304" t="s">
         <v>789</v>
-      </c>
-      <c r="B304" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
+        <v>790</v>
+      </c>
+      <c r="B305" t="s">
         <v>791</v>
       </c>
-      <c r="B305" t="s">
+      <c r="C305" t="s">
         <v>792</v>
-      </c>
-      <c r="C305" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
+        <v>793</v>
+      </c>
+      <c r="B306" t="s">
         <v>794</v>
-      </c>
-      <c r="B306" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
+        <v>795</v>
+      </c>
+      <c r="B307" t="s">
         <v>796</v>
-      </c>
-      <c r="B307" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
+        <v>797</v>
+      </c>
+      <c r="B308" t="s">
         <v>798</v>
       </c>
-      <c r="B308" t="s">
+      <c r="C308" t="s">
         <v>799</v>
-      </c>
-      <c r="C308" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
+        <v>800</v>
+      </c>
+      <c r="B309" t="s">
         <v>801</v>
       </c>
-      <c r="B309" t="s">
+      <c r="C309" t="s">
         <v>802</v>
-      </c>
-      <c r="C309" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>803</v>
+      </c>
+      <c r="B310" t="s">
         <v>804</v>
-      </c>
-      <c r="B310" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
+        <v>805</v>
+      </c>
+      <c r="B311" t="s">
         <v>806</v>
       </c>
-      <c r="B311" t="s">
+      <c r="C311" t="s">
         <v>807</v>
-      </c>
-      <c r="C311" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
+        <v>808</v>
+      </c>
+      <c r="B312" t="s">
         <v>809</v>
       </c>
-      <c r="B312" t="s">
+      <c r="C312" t="s">
         <v>810</v>
       </c>
-      <c r="C312" t="s">
+      <c r="D312" t="s">
         <v>811</v>
       </c>
-      <c r="D312" t="s">
+      <c r="E312" t="s">
         <v>812</v>
       </c>
-      <c r="E312" t="s">
+      <c r="F312" t="s">
         <v>813</v>
       </c>
-      <c r="F312" t="s">
+      <c r="G312" t="s">
         <v>814</v>
-      </c>
-      <c r="G312" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
+        <v>815</v>
+      </c>
+      <c r="B313" t="s">
         <v>816</v>
-      </c>
-      <c r="B313" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
+        <v>817</v>
+      </c>
+      <c r="B314" t="s">
         <v>818</v>
-      </c>
-      <c r="B314" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
+        <v>819</v>
+      </c>
+      <c r="B315" t="s">
         <v>820</v>
       </c>
-      <c r="B315" t="s">
-        <v>821</v>
+      <c r="C315" t="s">
+        <v>847</v>
+      </c>
+      <c r="D315" t="s">
+        <v>975</v>
+      </c>
+      <c r="E315" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
+        <v>821</v>
+      </c>
+      <c r="B316" t="s">
         <v>822</v>
       </c>
-      <c r="B316" t="s">
-        <v>823</v>
+      <c r="C316" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>823</v>
+      </c>
+      <c r="B317" t="s">
         <v>824</v>
       </c>
-      <c r="B317" t="s">
-        <v>825</v>
-      </c>
       <c r="C317" t="s">
-        <v>826</v>
+        <v>847</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B318" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B319" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B320" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B321" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B322" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B323" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>836</v>
+      </c>
+      <c r="B324" t="s">
+        <v>837</v>
+      </c>
+      <c r="C324" t="s">
         <v>838</v>
       </c>
-      <c r="B324" t="s">
+      <c r="D324" t="s">
         <v>839</v>
       </c>
-      <c r="C324" t="s">
+      <c r="E324" t="s">
         <v>840</v>
       </c>
-      <c r="D324" t="s">
+      <c r="F324" t="s">
         <v>841</v>
       </c>
-      <c r="E324" t="s">
+      <c r="G324" t="s">
         <v>842</v>
       </c>
-      <c r="F324" t="s">
+      <c r="H324" t="s">
         <v>843</v>
       </c>
-      <c r="G324" t="s">
+      <c r="I324" t="s">
         <v>844</v>
-      </c>
-      <c r="H324" t="s">
-        <v>845</v>
-      </c>
-      <c r="I324" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
+        <v>845</v>
+      </c>
+      <c r="B325" t="s">
+        <v>846</v>
+      </c>
+      <c r="C325" t="s">
         <v>847</v>
-      </c>
-      <c r="B325" t="s">
-        <v>848</v>
-      </c>
-      <c r="C325" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B326" t="s">
-        <v>851</v>
+        <v>849</v>
+      </c>
+      <c r="C326" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B327" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B328" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>854</v>
+      </c>
+      <c r="B329" t="s">
+        <v>855</v>
+      </c>
+      <c r="C329" t="s">
         <v>856</v>
-      </c>
-      <c r="B329" t="s">
-        <v>857</v>
-      </c>
-      <c r="C329" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B330" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
+        <v>863</v>
+      </c>
+      <c r="B332" t="s">
+        <v>864</v>
+      </c>
+      <c r="C332" t="s">
         <v>865</v>
-      </c>
-      <c r="B332" t="s">
-        <v>866</v>
-      </c>
-      <c r="C332" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
+        <v>866</v>
+      </c>
+      <c r="B333" t="s">
+        <v>867</v>
+      </c>
+      <c r="C333" t="s">
         <v>868</v>
-      </c>
-      <c r="B333" t="s">
-        <v>869</v>
-      </c>
-      <c r="C333" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>869</v>
+      </c>
+      <c r="B334" t="s">
+        <v>870</v>
+      </c>
+      <c r="C334" t="s">
         <v>871</v>
-      </c>
-      <c r="B334" t="s">
-        <v>872</v>
-      </c>
-      <c r="C334" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
+        <v>872</v>
+      </c>
+      <c r="B335" t="s">
+        <v>873</v>
+      </c>
+      <c r="C335" t="s">
         <v>874</v>
-      </c>
-      <c r="B335" t="s">
-        <v>875</v>
-      </c>
-      <c r="C335" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B336" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
+        <v>877</v>
+      </c>
+      <c r="B337" t="s">
+        <v>878</v>
+      </c>
+      <c r="C337" t="s">
         <v>879</v>
       </c>
-      <c r="B337" t="s">
+      <c r="D337" t="s">
         <v>880</v>
       </c>
-      <c r="C337" t="s">
-        <v>881</v>
-      </c>
-      <c r="D337" t="s">
-        <v>882</v>
-      </c>
       <c r="E337" t="s">
+        <v>969</v>
+      </c>
+      <c r="F337" t="s">
+        <v>970</v>
+      </c>
+      <c r="G337" t="s">
         <v>971</v>
       </c>
-      <c r="F337" t="s">
+      <c r="H337" t="s">
         <v>972</v>
       </c>
-      <c r="G337" t="s">
+      <c r="I337" t="s">
         <v>973</v>
-      </c>
-      <c r="H337" t="s">
-        <v>974</v>
-      </c>
-      <c r="I337" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B338" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
+        <v>883</v>
+      </c>
+      <c r="B339" t="s">
+        <v>884</v>
+      </c>
+      <c r="C339" t="s">
         <v>885</v>
-      </c>
-      <c r="B339" t="s">
-        <v>886</v>
-      </c>
-      <c r="C339" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
+        <v>886</v>
+      </c>
+      <c r="B340" t="s">
+        <v>887</v>
+      </c>
+      <c r="C340" t="s">
         <v>888</v>
-      </c>
-      <c r="B340" t="s">
-        <v>889</v>
-      </c>
-      <c r="C340" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
+        <v>889</v>
+      </c>
+      <c r="B341" t="s">
+        <v>890</v>
+      </c>
+      <c r="C341" t="s">
         <v>891</v>
-      </c>
-      <c r="B341" t="s">
-        <v>892</v>
-      </c>
-      <c r="C341" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B342" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B343" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
+        <v>896</v>
+      </c>
+      <c r="B344" t="s">
+        <v>897</v>
+      </c>
+      <c r="C344" t="s">
         <v>898</v>
-      </c>
-      <c r="B344" t="s">
-        <v>899</v>
-      </c>
-      <c r="C344" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
+        <v>899</v>
+      </c>
+      <c r="B345" t="s">
+        <v>900</v>
+      </c>
+      <c r="C345" t="s">
         <v>901</v>
-      </c>
-      <c r="B345" t="s">
-        <v>902</v>
-      </c>
-      <c r="C345" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
+        <v>902</v>
+      </c>
+      <c r="B346" t="s">
+        <v>903</v>
+      </c>
+      <c r="C346" t="s">
         <v>904</v>
-      </c>
-      <c r="B346" t="s">
-        <v>905</v>
-      </c>
-      <c r="C346" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B347" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
+        <v>907</v>
+      </c>
+      <c r="B348" t="s">
+        <v>908</v>
+      </c>
+      <c r="C348" t="s">
         <v>909</v>
       </c>
-      <c r="B348" t="s">
+      <c r="D348" t="s">
         <v>910</v>
-      </c>
-      <c r="C348" t="s">
-        <v>911</v>
-      </c>
-      <c r="D348" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B349" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B350" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B351" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
+        <v>917</v>
+      </c>
+      <c r="B352" t="s">
+        <v>918</v>
+      </c>
+      <c r="C352" t="s">
         <v>919</v>
       </c>
-      <c r="B352" t="s">
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
         <v>920</v>
       </c>
-      <c r="C352" t="s">
+      <c r="B353" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A353" t="s">
-        <v>922</v>
-      </c>
-      <c r="B353" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A354" t="s">
-        <v>923</v>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>306</v>
+      </c>
+      <c r="B355" t="s">
+        <v>977</v>
+      </c>
+      <c r="C355" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>577</v>
+      </c>
+      <c r="B356" t="s">
+        <v>578</v>
+      </c>
+      <c r="C356" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>886</v>
+      </c>
+      <c r="B357" t="s">
+        <v>887</v>
+      </c>
+      <c r="C357" t="s">
+        <v>888</v>
+      </c>
+      <c r="D357" t="s">
+        <v>980</v>
+      </c>
+      <c r="E357" t="s">
+        <v>981</v>
+      </c>
+      <c r="F357" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>983</v>
+      </c>
+      <c r="B358" t="s">
+        <v>984</v>
+      </c>
+      <c r="C358" t="s">
+        <v>985</v>
+      </c>
+      <c r="D358" t="s">
+        <v>986</v>
+      </c>
+      <c r="E358" t="s">
+        <v>987</v>
+      </c>
+      <c r="F358" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>989</v>
+      </c>
+      <c r="B359" t="s">
+        <v>990</v>
+      </c>
+      <c r="C359" t="s">
+        <v>991</v>
+      </c>
+      <c r="D359" t="s">
+        <v>992</v>
+      </c>
+      <c r="E359" t="s">
+        <v>993</v>
+      </c>
+      <c r="F359" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G359" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>995</v>
+      </c>
+      <c r="B360" t="s">
+        <v>994</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E360" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F360" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G360" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>996</v>
+      </c>
+      <c r="B361" t="s">
+        <v>996</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D361" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E361" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F361" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>997</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>998</v>
+      </c>
+      <c r="B363" t="s">
+        <v>999</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>